<commit_message>
Rewrote the `debug()` function for Excel service
</commit_message>
<xml_diff>
--- a/docs/services/spreadsheets/needs.xlsx
+++ b/docs/services/spreadsheets/needs.xlsx
@@ -63,7 +63,7 @@
     <t>progress</t>
   </si>
   <si>
-    <t xml:space="preserve">Celestina Duodu</t>
+    <t xml:space="preserve">Haiyang Zhang</t>
   </si>
   <si>
     <t xml:space="preserve">Import from Excel 4</t>
@@ -733,7 +733,7 @@
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
@@ -756,7 +756,7 @@
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
@@ -779,7 +779,7 @@
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -802,7 +802,7 @@
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -825,7 +825,7 @@
       <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -848,13 +848,13 @@
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="1">
@@ -871,7 +871,7 @@
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -894,7 +894,7 @@
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -917,7 +917,7 @@
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -940,13 +940,13 @@
       <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="1">
@@ -963,7 +963,7 @@
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -986,7 +986,7 @@
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1009,7 +1009,7 @@
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1032,13 +1032,13 @@
       <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F16" s="1">
@@ -1055,7 +1055,7 @@
       <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1078,7 +1078,7 @@
       <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1101,7 +1101,7 @@
       <c r="B19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1124,13 +1124,13 @@
       <c r="B20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="1">
@@ -1147,7 +1147,7 @@
       <c r="B21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -1166,7 +1166,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>